<commit_message>
fix line in change log
</commit_message>
<xml_diff>
--- a/Change_log_for_SS_3.30.xlsx
+++ b/Change_log_for_SS_3.30.xlsx
@@ -2157,27 +2157,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>forecast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:  fix, and augment control of, the continue last dev feature</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>output</t>
     </r>
     <r>
@@ -2569,6 +2548,27 @@
         <family val="2"/>
       </rPr>
       <t>: provide std.err. for time series of summary biomass, see Extra_Std input options</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>:  fix read error for mean weight-at-age data</t>
     </r>
   </si>
 </sst>
@@ -2871,7 +2871,7 @@
   <dimension ref="A1:Z1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2952,7 +2952,7 @@
         <v>44322</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>383</v>
@@ -2979,7 +2979,7 @@
         <v>44316</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>394</v>
@@ -3006,7 +3006,7 @@
         <v>44299</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>384</v>
@@ -3033,7 +3033,7 @@
         <v>44291</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>402</v>
@@ -3060,7 +3060,7 @@
         <v>44285</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>382</v>
@@ -3087,7 +3087,7 @@
         <v>44277</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>396</v>
@@ -3114,7 +3114,7 @@
         <v>44273</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>380</v>
@@ -3141,7 +3141,7 @@
         <v>44272</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>397</v>
@@ -3168,7 +3168,7 @@
         <v>44272</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>381</v>
@@ -3195,7 +3195,7 @@
         <v>44267</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>406</v>
@@ -3222,7 +3222,7 @@
         <v>44266</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>398</v>
@@ -3249,7 +3249,7 @@
         <v>44266</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>379</v>
@@ -3276,7 +3276,7 @@
         <v>44264</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>399</v>
@@ -3288,7 +3288,7 @@
         <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>30</v>
@@ -3303,7 +3303,7 @@
         <v>44260</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>378</v>
@@ -3330,7 +3330,7 @@
         <v>44236</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>377</v>
@@ -3357,7 +3357,7 @@
         <v>44232</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>404</v>
@@ -3384,7 +3384,7 @@
         <v>44223</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>401</v>
@@ -3411,7 +3411,7 @@
         <v>44222</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>375</v>
@@ -3438,7 +3438,7 @@
         <v>44186</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>373</v>
@@ -3546,7 +3546,7 @@
         <v>44140</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>418</v>
+        <v>438</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>369</v>

</xml_diff>

<commit_message>
update change log date of release
</commit_message>
<xml_diff>
--- a/Change_log_for_SS_3.30.xlsx
+++ b/Change_log_for_SS_3.30.xlsx
@@ -2871,7 +2871,7 @@
   <dimension ref="A1:Z1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2922,7 +2922,7 @@
         <v>391</v>
       </c>
       <c r="B2" s="5">
-        <v>44341</v>
+        <v>44358</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>392</v>

</xml_diff>